<commit_message>
smol changes and fixes
</commit_message>
<xml_diff>
--- a/Horarios.xlsx
+++ b/Horarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="IC1" sheetId="1" state="visible" r:id="rId2"/>
@@ -400,11 +400,11 @@
   </sheetPr>
   <dimension ref="A1:AK35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.05"/>
   </cols>
@@ -3875,11 +3875,11 @@
   </sheetPr>
   <dimension ref="A1:AQ23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
   </cols>
@@ -6714,7 +6714,7 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7694,7 +7694,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8772,7 +8772,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.22"/>
   </cols>
@@ -9769,7 +9769,7 @@
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -12633,7 +12633,7 @@
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.16"/>
   </cols>
@@ -13273,7 +13273,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.37"/>
   </cols>
@@ -16342,7 +16342,7 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -17200,7 +17200,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
horarios2trenes acepta horarios que pueden saltar paradas
</commit_message>
<xml_diff>
--- a/Horarios.xlsx
+++ b/Horarios.xlsx
@@ -350,7 +350,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -391,6 +391,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3234,10 +3238,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AQ23"/>
+  <dimension ref="A1:AQ24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3245,24 +3249,38 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.31"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="B1" s="10" t="n">
+        <v>43</v>
+      </c>
+      <c r="C1" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D1" s="10" t="n">
+        <v>11</v>
+      </c>
+      <c r="E1" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F1" s="10" t="n">
+        <v>39</v>
+      </c>
+      <c r="G1" s="10" t="n">
+        <v>17</v>
+      </c>
+      <c r="H1" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
@@ -3293,2253 +3311,2302 @@
       <c r="AQ1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="3"/>
+      <c r="AO2" s="3"/>
+      <c r="AP2" s="3"/>
+      <c r="AQ2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AN2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AP2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AQ2" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="7" t="n">
-        <v>520</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>522</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>555</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>556</v>
-      </c>
-      <c r="F3" s="7" t="n">
-        <v>655</v>
-      </c>
-      <c r="G3" s="7" t="n">
-        <v>656</v>
-      </c>
-      <c r="H3" s="7" t="n">
-        <v>725</v>
-      </c>
-      <c r="I3" s="7" t="n">
-        <v>728</v>
-      </c>
-      <c r="J3" s="7" t="n">
-        <v>755</v>
-      </c>
-      <c r="K3" s="7" t="n">
-        <v>756</v>
-      </c>
-      <c r="L3" s="7" t="n">
-        <v>855</v>
-      </c>
-      <c r="M3" s="7" t="n">
-        <v>856</v>
-      </c>
-      <c r="N3" s="7" t="n">
-        <v>925</v>
-      </c>
-      <c r="O3" s="7" t="n">
-        <v>928</v>
-      </c>
-      <c r="P3" s="7" t="n">
-        <v>955</v>
-      </c>
-      <c r="Q3" s="7" t="n">
-        <v>956</v>
-      </c>
-      <c r="R3" s="7" t="n">
-        <v>1125</v>
-      </c>
-      <c r="S3" s="7" t="n">
-        <v>1128</v>
-      </c>
-      <c r="T3" s="7" t="n">
-        <v>1125</v>
-      </c>
-      <c r="U3" s="7" t="n">
-        <v>1128</v>
-      </c>
-      <c r="V3" s="7" t="n">
-        <v>1255</v>
-      </c>
-      <c r="W3" s="7" t="n">
-        <v>1256</v>
-      </c>
-      <c r="X3" s="7" t="n">
-        <v>1325</v>
-      </c>
-      <c r="Y3" s="7" t="n">
-        <v>1328</v>
-      </c>
-      <c r="Z3" s="7" t="n">
-        <v>1455</v>
-      </c>
-      <c r="AA3" s="7" t="n">
-        <v>1456</v>
-      </c>
-      <c r="AB3" s="7" t="n">
-        <v>1525</v>
-      </c>
-      <c r="AC3" s="7" t="n">
-        <v>1528</v>
-      </c>
-      <c r="AD3" s="7" t="n">
-        <v>1555</v>
-      </c>
-      <c r="AE3" s="7" t="n">
-        <v>1556</v>
-      </c>
-      <c r="AF3" s="7" t="n">
-        <v>1655</v>
-      </c>
-      <c r="AG3" s="7" t="n">
-        <v>1656</v>
-      </c>
-      <c r="AH3" s="7" t="n">
-        <v>1825</v>
-      </c>
-      <c r="AI3" s="7" t="n">
-        <v>1828</v>
-      </c>
-      <c r="AJ3" s="7" t="n">
-        <v>1855</v>
-      </c>
-      <c r="AK3" s="7" t="n">
-        <v>1856</v>
-      </c>
-      <c r="AL3" s="7" t="n">
-        <v>2055</v>
-      </c>
-      <c r="AM3" s="7" t="n">
-        <v>2056</v>
-      </c>
-      <c r="AN3" s="7" t="n">
-        <v>2155</v>
-      </c>
-      <c r="AO3" s="7" t="n">
-        <v>2156</v>
-      </c>
-      <c r="AP3" s="7" t="n">
-        <v>2225</v>
-      </c>
-      <c r="AQ3" s="7" t="n">
-        <v>2228</v>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ3" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="B4" s="7" t="n">
-        <v>532</v>
+        <v>520</v>
       </c>
       <c r="C4" s="7" t="n">
-        <v>533</v>
+        <v>522</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>606</v>
+        <v>555</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>607</v>
+        <v>556</v>
       </c>
       <c r="F4" s="7" t="n">
-        <v>706</v>
+        <v>655</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>707</v>
-      </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+        <v>656</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>725</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>728</v>
+      </c>
       <c r="J4" s="7" t="n">
-        <v>806</v>
+        <v>755</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>807</v>
+        <v>756</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>906</v>
+        <v>855</v>
       </c>
       <c r="M4" s="7" t="n">
-        <v>907</v>
-      </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
+        <v>856</v>
+      </c>
+      <c r="N4" s="7" t="n">
+        <v>925</v>
+      </c>
+      <c r="O4" s="7" t="n">
+        <v>928</v>
+      </c>
       <c r="P4" s="7" t="n">
-        <v>1006</v>
+        <v>955</v>
       </c>
       <c r="Q4" s="7" t="n">
-        <v>1007</v>
-      </c>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
+        <v>956</v>
+      </c>
+      <c r="R4" s="7" t="n">
+        <v>1125</v>
+      </c>
+      <c r="S4" s="7" t="n">
+        <v>1128</v>
+      </c>
+      <c r="T4" s="7" t="n">
+        <v>1125</v>
+      </c>
+      <c r="U4" s="7" t="n">
+        <v>1128</v>
+      </c>
       <c r="V4" s="7" t="n">
-        <v>1306</v>
+        <v>1255</v>
       </c>
       <c r="W4" s="7" t="n">
-        <v>1307</v>
-      </c>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
+        <v>1256</v>
+      </c>
+      <c r="X4" s="7" t="n">
+        <v>1325</v>
+      </c>
+      <c r="Y4" s="7" t="n">
+        <v>1328</v>
+      </c>
       <c r="Z4" s="7" t="n">
-        <v>1506</v>
+        <v>1455</v>
       </c>
       <c r="AA4" s="7" t="n">
-        <v>1507</v>
-      </c>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7"/>
+        <v>1456</v>
+      </c>
+      <c r="AB4" s="7" t="n">
+        <v>1525</v>
+      </c>
+      <c r="AC4" s="7" t="n">
+        <v>1528</v>
+      </c>
       <c r="AD4" s="7" t="n">
-        <v>1606</v>
+        <v>1555</v>
       </c>
       <c r="AE4" s="7" t="n">
-        <v>1607</v>
+        <v>1556</v>
       </c>
       <c r="AF4" s="7" t="n">
-        <v>1706</v>
+        <v>1655</v>
       </c>
       <c r="AG4" s="7" t="n">
-        <v>1707</v>
-      </c>
-      <c r="AH4" s="7"/>
-      <c r="AI4" s="7"/>
+        <v>1656</v>
+      </c>
+      <c r="AH4" s="7" t="n">
+        <v>1825</v>
+      </c>
+      <c r="AI4" s="7" t="n">
+        <v>1828</v>
+      </c>
       <c r="AJ4" s="7" t="n">
-        <v>1906</v>
+        <v>1855</v>
       </c>
       <c r="AK4" s="7" t="n">
-        <v>1907</v>
+        <v>1856</v>
       </c>
       <c r="AL4" s="7" t="n">
-        <v>2106</v>
+        <v>2055</v>
       </c>
       <c r="AM4" s="7" t="n">
-        <v>2107</v>
+        <v>2056</v>
       </c>
       <c r="AN4" s="7" t="n">
-        <v>2206</v>
+        <v>2155</v>
       </c>
       <c r="AO4" s="7" t="n">
-        <v>2207</v>
+        <v>2156</v>
       </c>
       <c r="AP4" s="7" t="n">
-        <v>400</v>
+        <v>2225</v>
       </c>
       <c r="AQ4" s="7" t="n">
-        <v>400</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="B5" s="7" t="n">
-        <v>554</v>
+        <v>532</v>
       </c>
       <c r="C5" s="7" t="n">
-        <v>558</v>
+        <v>533</v>
       </c>
       <c r="D5" s="7" t="n">
-        <v>625</v>
+        <v>606</v>
       </c>
       <c r="E5" s="7" t="n">
-        <v>629</v>
+        <v>607</v>
       </c>
       <c r="F5" s="7" t="n">
-        <v>725</v>
+        <v>706</v>
       </c>
       <c r="G5" s="7" t="n">
-        <v>729</v>
-      </c>
-      <c r="H5" s="7" t="n">
-        <v>755</v>
-      </c>
-      <c r="I5" s="7" t="n">
-        <v>758</v>
-      </c>
+        <v>707</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
       <c r="J5" s="7" t="n">
-        <v>825</v>
+        <v>806</v>
       </c>
       <c r="K5" s="7" t="n">
-        <v>829</v>
+        <v>807</v>
       </c>
       <c r="L5" s="7" t="n">
-        <v>925</v>
+        <v>906</v>
       </c>
       <c r="M5" s="7" t="n">
-        <v>929</v>
-      </c>
-      <c r="N5" s="7" t="n">
-        <v>955</v>
-      </c>
-      <c r="O5" s="7" t="n">
-        <v>958</v>
-      </c>
+        <v>907</v>
+      </c>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
       <c r="P5" s="7" t="n">
-        <v>1025</v>
+        <v>1006</v>
       </c>
       <c r="Q5" s="7" t="n">
-        <v>1029</v>
-      </c>
-      <c r="R5" s="7" t="n">
-        <v>1155</v>
-      </c>
-      <c r="S5" s="7" t="n">
-        <v>1158</v>
-      </c>
-      <c r="T5" s="7" t="n">
-        <v>1155</v>
-      </c>
-      <c r="U5" s="7" t="n">
-        <v>1158</v>
-      </c>
+        <v>1007</v>
+      </c>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
       <c r="V5" s="7" t="n">
-        <v>1325</v>
+        <v>1306</v>
       </c>
       <c r="W5" s="7" t="n">
-        <v>1329</v>
-      </c>
-      <c r="X5" s="7" t="n">
-        <v>1355</v>
-      </c>
-      <c r="Y5" s="7" t="n">
-        <v>1358</v>
-      </c>
+        <v>1307</v>
+      </c>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
       <c r="Z5" s="7" t="n">
-        <v>1525</v>
+        <v>1506</v>
       </c>
       <c r="AA5" s="7" t="n">
-        <v>1529</v>
-      </c>
-      <c r="AB5" s="7" t="n">
-        <v>1555</v>
-      </c>
-      <c r="AC5" s="7" t="n">
-        <v>1558</v>
-      </c>
+        <v>1507</v>
+      </c>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
       <c r="AD5" s="7" t="n">
-        <v>1625</v>
+        <v>1606</v>
       </c>
       <c r="AE5" s="7" t="n">
-        <v>1629</v>
+        <v>1607</v>
       </c>
       <c r="AF5" s="7" t="n">
-        <v>1725</v>
+        <v>1706</v>
       </c>
       <c r="AG5" s="7" t="n">
-        <v>1729</v>
-      </c>
-      <c r="AH5" s="7" t="n">
-        <v>1855</v>
-      </c>
-      <c r="AI5" s="7" t="n">
-        <v>1858</v>
-      </c>
+        <v>1707</v>
+      </c>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
       <c r="AJ5" s="7" t="n">
-        <v>1925</v>
+        <v>1906</v>
       </c>
       <c r="AK5" s="7" t="n">
-        <v>1929</v>
+        <v>1907</v>
       </c>
       <c r="AL5" s="7" t="n">
-        <v>2125</v>
+        <v>2106</v>
       </c>
       <c r="AM5" s="7" t="n">
-        <v>2129</v>
+        <v>2107</v>
       </c>
       <c r="AN5" s="7" t="n">
-        <v>2225</v>
+        <v>2206</v>
       </c>
       <c r="AO5" s="7" t="n">
-        <v>2229</v>
+        <v>2207</v>
       </c>
       <c r="AP5" s="7" t="n">
-        <v>2255</v>
+        <f aca="false">AN5+200</f>
+        <v>2406</v>
       </c>
       <c r="AQ5" s="7" t="n">
-        <v>2258</v>
+        <f aca="false">AO5+200</f>
+        <v>2407</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B6" s="7" t="n">
-        <v>626</v>
+        <v>554</v>
       </c>
       <c r="C6" s="7" t="n">
-        <v>634</v>
+        <v>558</v>
       </c>
       <c r="D6" s="7" t="n">
-        <v>656</v>
+        <v>625</v>
       </c>
       <c r="E6" s="7" t="n">
-        <v>704</v>
+        <v>629</v>
       </c>
       <c r="F6" s="7" t="n">
-        <v>756</v>
+        <v>725</v>
       </c>
       <c r="G6" s="7" t="n">
-        <v>804</v>
+        <v>729</v>
       </c>
       <c r="H6" s="7" t="n">
-        <v>826</v>
+        <v>755</v>
       </c>
       <c r="I6" s="7" t="n">
-        <v>834</v>
+        <v>758</v>
       </c>
       <c r="J6" s="7" t="n">
-        <v>856</v>
+        <v>825</v>
       </c>
       <c r="K6" s="7" t="n">
-        <v>904</v>
+        <v>829</v>
       </c>
       <c r="L6" s="7" t="n">
-        <v>956</v>
+        <v>925</v>
       </c>
       <c r="M6" s="7" t="n">
-        <v>1004</v>
+        <v>929</v>
       </c>
       <c r="N6" s="7" t="n">
-        <v>1026</v>
+        <v>955</v>
       </c>
       <c r="O6" s="7" t="n">
-        <v>1034</v>
+        <v>958</v>
       </c>
       <c r="P6" s="7" t="n">
-        <v>1056</v>
+        <v>1025</v>
       </c>
       <c r="Q6" s="7" t="n">
-        <v>1104</v>
+        <v>1029</v>
       </c>
       <c r="R6" s="7" t="n">
-        <v>1226</v>
+        <v>1155</v>
       </c>
       <c r="S6" s="7" t="n">
-        <v>1234</v>
+        <v>1158</v>
       </c>
       <c r="T6" s="7" t="n">
-        <v>1226</v>
+        <v>1155</v>
       </c>
       <c r="U6" s="7" t="n">
-        <v>1234</v>
+        <v>1158</v>
       </c>
       <c r="V6" s="7" t="n">
-        <v>1356</v>
+        <v>1325</v>
       </c>
       <c r="W6" s="7" t="n">
-        <v>1404</v>
+        <v>1329</v>
       </c>
       <c r="X6" s="7" t="n">
-        <v>1426</v>
+        <v>1355</v>
       </c>
       <c r="Y6" s="7" t="n">
-        <v>1434</v>
+        <v>1358</v>
       </c>
       <c r="Z6" s="7" t="n">
-        <v>1556</v>
+        <v>1525</v>
       </c>
       <c r="AA6" s="7" t="n">
-        <v>1604</v>
+        <v>1529</v>
       </c>
       <c r="AB6" s="7" t="n">
-        <v>1626</v>
+        <v>1555</v>
       </c>
       <c r="AC6" s="7" t="n">
-        <v>1634</v>
+        <v>1558</v>
       </c>
       <c r="AD6" s="7" t="n">
-        <v>1656</v>
+        <v>1625</v>
       </c>
       <c r="AE6" s="7" t="n">
-        <v>1704</v>
+        <v>1629</v>
       </c>
       <c r="AF6" s="7" t="n">
-        <v>1756</v>
+        <v>1725</v>
       </c>
       <c r="AG6" s="7" t="n">
-        <v>1804</v>
+        <v>1729</v>
       </c>
       <c r="AH6" s="7" t="n">
-        <v>1926</v>
+        <v>1855</v>
       </c>
       <c r="AI6" s="7" t="n">
-        <v>1934</v>
+        <v>1858</v>
       </c>
       <c r="AJ6" s="7" t="n">
-        <v>1956</v>
+        <v>1925</v>
       </c>
       <c r="AK6" s="7" t="n">
-        <v>2004</v>
+        <v>1929</v>
       </c>
       <c r="AL6" s="7" t="n">
-        <v>2156</v>
+        <v>2125</v>
       </c>
       <c r="AM6" s="7" t="n">
-        <v>2204</v>
+        <v>2129</v>
       </c>
       <c r="AN6" s="7" t="n">
-        <v>2256</v>
+        <v>2225</v>
       </c>
       <c r="AO6" s="7" t="n">
-        <v>2304</v>
+        <v>2229</v>
       </c>
       <c r="AP6" s="7" t="n">
-        <v>2326</v>
+        <v>2255</v>
       </c>
       <c r="AQ6" s="7" t="n">
-        <v>2334</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B7" s="7" t="n">
-        <v>652</v>
+        <v>626</v>
       </c>
       <c r="C7" s="7" t="n">
-        <v>654</v>
+        <v>634</v>
       </c>
       <c r="D7" s="7" t="n">
-        <v>723</v>
+        <v>656</v>
       </c>
       <c r="E7" s="7" t="n">
-        <v>724</v>
+        <v>704</v>
       </c>
       <c r="F7" s="7" t="n">
-        <v>823</v>
+        <v>756</v>
       </c>
       <c r="G7" s="7" t="n">
-        <v>824</v>
+        <v>804</v>
       </c>
       <c r="H7" s="7" t="n">
-        <v>852</v>
+        <v>826</v>
       </c>
       <c r="I7" s="7" t="n">
-        <v>854</v>
+        <v>834</v>
       </c>
       <c r="J7" s="7" t="n">
-        <v>923</v>
+        <v>856</v>
       </c>
       <c r="K7" s="7" t="n">
-        <v>924</v>
+        <v>904</v>
       </c>
       <c r="L7" s="7" t="n">
-        <v>1023</v>
+        <v>956</v>
       </c>
       <c r="M7" s="7" t="n">
-        <v>1024</v>
+        <v>1004</v>
       </c>
       <c r="N7" s="7" t="n">
-        <v>1052</v>
+        <v>1026</v>
       </c>
       <c r="O7" s="7" t="n">
-        <v>1054</v>
+        <v>1034</v>
       </c>
       <c r="P7" s="7" t="n">
-        <v>1123</v>
+        <v>1056</v>
       </c>
       <c r="Q7" s="7" t="n">
-        <v>1124</v>
+        <v>1104</v>
       </c>
       <c r="R7" s="7" t="n">
-        <v>1252</v>
+        <v>1226</v>
       </c>
       <c r="S7" s="7" t="n">
-        <v>1254</v>
+        <v>1234</v>
       </c>
       <c r="T7" s="7" t="n">
-        <v>1252</v>
+        <v>1226</v>
       </c>
       <c r="U7" s="7" t="n">
-        <v>1254</v>
+        <v>1234</v>
       </c>
       <c r="V7" s="7" t="n">
-        <v>1423</v>
+        <v>1356</v>
       </c>
       <c r="W7" s="7" t="n">
-        <v>1424</v>
+        <v>1404</v>
       </c>
       <c r="X7" s="7" t="n">
-        <v>1452</v>
+        <v>1426</v>
       </c>
       <c r="Y7" s="7" t="n">
-        <v>1454</v>
+        <v>1434</v>
       </c>
       <c r="Z7" s="7" t="n">
-        <v>1623</v>
+        <v>1556</v>
       </c>
       <c r="AA7" s="7" t="n">
-        <v>1624</v>
+        <v>1604</v>
       </c>
       <c r="AB7" s="7" t="n">
-        <v>1652</v>
+        <v>1626</v>
       </c>
       <c r="AC7" s="7" t="n">
-        <v>1654</v>
+        <v>1634</v>
       </c>
       <c r="AD7" s="7" t="n">
-        <v>1723</v>
+        <v>1656</v>
       </c>
       <c r="AE7" s="7" t="n">
-        <v>1724</v>
+        <v>1704</v>
       </c>
       <c r="AF7" s="7" t="n">
-        <v>1823</v>
+        <v>1756</v>
       </c>
       <c r="AG7" s="7" t="n">
-        <v>1824</v>
+        <v>1804</v>
       </c>
       <c r="AH7" s="7" t="n">
-        <v>1952</v>
+        <v>1926</v>
       </c>
       <c r="AI7" s="7" t="n">
-        <v>1954</v>
+        <v>1934</v>
       </c>
       <c r="AJ7" s="7" t="n">
-        <v>2023</v>
+        <v>1956</v>
       </c>
       <c r="AK7" s="7" t="n">
-        <v>2024</v>
+        <v>2004</v>
       </c>
       <c r="AL7" s="7" t="n">
-        <v>2223</v>
+        <v>2156</v>
       </c>
       <c r="AM7" s="7" t="n">
-        <v>2224</v>
+        <v>2204</v>
       </c>
       <c r="AN7" s="7" t="n">
-        <v>2323</v>
+        <v>2256</v>
       </c>
       <c r="AO7" s="7" t="n">
-        <v>2324</v>
+        <v>2304</v>
       </c>
       <c r="AP7" s="7" t="n">
-        <v>2352</v>
+        <v>2326</v>
       </c>
       <c r="AQ7" s="7" t="n">
-        <v>2354</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="7" t="n">
-        <v>703</v>
+        <v>652</v>
       </c>
       <c r="C8" s="7" t="n">
-        <v>704</v>
+        <v>654</v>
       </c>
       <c r="D8" s="7" t="n">
-        <v>733</v>
+        <v>723</v>
       </c>
       <c r="E8" s="7" t="n">
-        <v>734</v>
+        <v>724</v>
       </c>
       <c r="F8" s="7" t="n">
-        <v>833</v>
+        <v>823</v>
       </c>
       <c r="G8" s="7" t="n">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="H8" s="7" t="n">
-        <v>903</v>
+        <v>852</v>
       </c>
       <c r="I8" s="7" t="n">
-        <v>904</v>
+        <v>854</v>
       </c>
       <c r="J8" s="7" t="n">
-        <v>933</v>
+        <v>923</v>
       </c>
       <c r="K8" s="7" t="n">
-        <v>934</v>
+        <v>924</v>
       </c>
       <c r="L8" s="7" t="n">
-        <v>1033</v>
+        <v>1023</v>
       </c>
       <c r="M8" s="7" t="n">
-        <v>1034</v>
+        <v>1024</v>
       </c>
       <c r="N8" s="7" t="n">
-        <v>1103</v>
+        <v>1052</v>
       </c>
       <c r="O8" s="7" t="n">
-        <v>1104</v>
+        <v>1054</v>
       </c>
       <c r="P8" s="7" t="n">
-        <v>1133</v>
+        <v>1123</v>
       </c>
       <c r="Q8" s="7" t="n">
-        <v>1134</v>
+        <v>1124</v>
       </c>
       <c r="R8" s="7" t="n">
-        <v>1303</v>
+        <v>1252</v>
       </c>
       <c r="S8" s="7" t="n">
-        <v>1304</v>
+        <v>1254</v>
       </c>
       <c r="T8" s="7" t="n">
-        <v>1303</v>
+        <v>1252</v>
       </c>
       <c r="U8" s="7" t="n">
-        <v>1304</v>
+        <v>1254</v>
       </c>
       <c r="V8" s="7" t="n">
-        <v>1433</v>
+        <v>1423</v>
       </c>
       <c r="W8" s="7" t="n">
-        <v>1434</v>
+        <v>1424</v>
       </c>
       <c r="X8" s="7" t="n">
-        <v>1503</v>
+        <v>1452</v>
       </c>
       <c r="Y8" s="7" t="n">
-        <v>1504</v>
+        <v>1454</v>
       </c>
       <c r="Z8" s="7" t="n">
-        <v>1633</v>
+        <v>1623</v>
       </c>
       <c r="AA8" s="7" t="n">
-        <v>1634</v>
+        <v>1624</v>
       </c>
       <c r="AB8" s="7" t="n">
-        <v>1703</v>
+        <v>1652</v>
       </c>
       <c r="AC8" s="7" t="n">
-        <v>1704</v>
+        <v>1654</v>
       </c>
       <c r="AD8" s="7" t="n">
-        <v>1733</v>
+        <v>1723</v>
       </c>
       <c r="AE8" s="7" t="n">
-        <v>1734</v>
+        <v>1724</v>
       </c>
       <c r="AF8" s="7" t="n">
-        <v>1833</v>
+        <v>1823</v>
       </c>
       <c r="AG8" s="7" t="n">
-        <v>1834</v>
+        <v>1824</v>
       </c>
       <c r="AH8" s="7" t="n">
-        <v>2003</v>
+        <v>1952</v>
       </c>
       <c r="AI8" s="7" t="n">
-        <v>2004</v>
+        <v>1954</v>
       </c>
       <c r="AJ8" s="7" t="n">
-        <v>2033</v>
+        <v>2023</v>
       </c>
       <c r="AK8" s="7" t="n">
-        <v>2034</v>
+        <v>2024</v>
       </c>
       <c r="AL8" s="7" t="n">
-        <v>2233</v>
+        <v>2223</v>
       </c>
       <c r="AM8" s="7" t="n">
-        <v>2234</v>
+        <v>2224</v>
       </c>
       <c r="AN8" s="7" t="n">
-        <v>2333</v>
+        <v>2323</v>
       </c>
       <c r="AO8" s="7" t="n">
-        <v>2334</v>
+        <v>2324</v>
       </c>
       <c r="AP8" s="7" t="n">
-        <v>2403</v>
+        <v>2352</v>
       </c>
       <c r="AQ8" s="7" t="n">
-        <v>2404</v>
+        <v>2354</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>703</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>704</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>733</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>734</v>
+      </c>
+      <c r="F9" s="7" t="n">
+        <v>833</v>
+      </c>
+      <c r="G9" s="7" t="n">
+        <v>834</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>903</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <v>904</v>
+      </c>
+      <c r="J9" s="7" t="n">
+        <v>933</v>
+      </c>
+      <c r="K9" s="7" t="n">
+        <v>934</v>
+      </c>
+      <c r="L9" s="7" t="n">
+        <v>1033</v>
+      </c>
+      <c r="M9" s="7" t="n">
+        <v>1034</v>
+      </c>
+      <c r="N9" s="7" t="n">
+        <v>1103</v>
+      </c>
+      <c r="O9" s="7" t="n">
+        <v>1104</v>
+      </c>
+      <c r="P9" s="7" t="n">
+        <v>1133</v>
+      </c>
+      <c r="Q9" s="7" t="n">
+        <v>1134</v>
+      </c>
+      <c r="R9" s="7" t="n">
+        <v>1303</v>
+      </c>
+      <c r="S9" s="7" t="n">
+        <v>1304</v>
+      </c>
+      <c r="T9" s="7" t="n">
+        <v>1303</v>
+      </c>
+      <c r="U9" s="7" t="n">
+        <v>1304</v>
+      </c>
+      <c r="V9" s="7" t="n">
+        <v>1433</v>
+      </c>
+      <c r="W9" s="7" t="n">
+        <v>1434</v>
+      </c>
+      <c r="X9" s="7" t="n">
+        <v>1503</v>
+      </c>
+      <c r="Y9" s="7" t="n">
+        <v>1504</v>
+      </c>
+      <c r="Z9" s="7" t="n">
+        <v>1633</v>
+      </c>
+      <c r="AA9" s="7" t="n">
+        <v>1634</v>
+      </c>
+      <c r="AB9" s="7" t="n">
+        <v>1703</v>
+      </c>
+      <c r="AC9" s="7" t="n">
+        <v>1704</v>
+      </c>
+      <c r="AD9" s="7" t="n">
+        <v>1733</v>
+      </c>
+      <c r="AE9" s="7" t="n">
+        <v>1734</v>
+      </c>
+      <c r="AF9" s="7" t="n">
+        <v>1833</v>
+      </c>
+      <c r="AG9" s="7" t="n">
+        <v>1834</v>
+      </c>
+      <c r="AH9" s="7" t="n">
+        <v>2003</v>
+      </c>
+      <c r="AI9" s="7" t="n">
+        <v>2004</v>
+      </c>
+      <c r="AJ9" s="7" t="n">
+        <v>2033</v>
+      </c>
+      <c r="AK9" s="7" t="n">
+        <v>2034</v>
+      </c>
+      <c r="AL9" s="7" t="n">
+        <v>2233</v>
+      </c>
+      <c r="AM9" s="7" t="n">
+        <v>2234</v>
+      </c>
+      <c r="AN9" s="7" t="n">
+        <v>2333</v>
+      </c>
+      <c r="AO9" s="7" t="n">
+        <v>2334</v>
+      </c>
+      <c r="AP9" s="7" t="n">
+        <v>2403</v>
+      </c>
+      <c r="AQ9" s="7" t="n">
+        <v>2404</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="7" t="n">
+      <c r="B10" s="7" t="n">
         <v>722</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C10" s="7" t="n">
         <v>723</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D10" s="7" t="n">
         <v>751</v>
       </c>
-      <c r="E9" s="7" t="n">
+      <c r="E10" s="7" t="n">
         <v>753</v>
       </c>
-      <c r="F9" s="7" t="n">
+      <c r="F10" s="7" t="n">
         <v>851</v>
       </c>
-      <c r="G9" s="7" t="n">
+      <c r="G10" s="7" t="n">
         <v>853</v>
       </c>
-      <c r="H9" s="7" t="n">
+      <c r="H10" s="7" t="n">
         <v>922</v>
       </c>
-      <c r="I9" s="7" t="n">
+      <c r="I10" s="7" t="n">
         <v>923</v>
       </c>
-      <c r="J9" s="7" t="n">
+      <c r="J10" s="7" t="n">
         <v>951</v>
       </c>
-      <c r="K9" s="7" t="n">
+      <c r="K10" s="7" t="n">
         <v>953</v>
       </c>
-      <c r="L9" s="7" t="n">
+      <c r="L10" s="7" t="n">
         <v>1051</v>
       </c>
-      <c r="M9" s="7" t="n">
+      <c r="M10" s="7" t="n">
         <v>1053</v>
       </c>
-      <c r="N9" s="7" t="n">
+      <c r="N10" s="7" t="n">
         <v>1122</v>
       </c>
-      <c r="O9" s="7" t="n">
+      <c r="O10" s="7" t="n">
         <v>1123</v>
       </c>
-      <c r="P9" s="7" t="n">
+      <c r="P10" s="7" t="n">
         <v>1151</v>
       </c>
-      <c r="Q9" s="7" t="n">
+      <c r="Q10" s="7" t="n">
         <v>1153</v>
       </c>
-      <c r="R9" s="7" t="n">
+      <c r="R10" s="7" t="n">
         <v>1322</v>
       </c>
-      <c r="S9" s="7" t="n">
+      <c r="S10" s="7" t="n">
         <v>1323</v>
       </c>
-      <c r="T9" s="7" t="n">
+      <c r="T10" s="7" t="n">
         <v>1322</v>
       </c>
-      <c r="U9" s="7" t="n">
+      <c r="U10" s="7" t="n">
         <v>1323</v>
       </c>
-      <c r="V9" s="7" t="n">
+      <c r="V10" s="7" t="n">
         <v>1451</v>
       </c>
-      <c r="W9" s="7" t="n">
+      <c r="W10" s="7" t="n">
         <v>1453</v>
       </c>
-      <c r="X9" s="7" t="n">
+      <c r="X10" s="7" t="n">
         <v>1522</v>
       </c>
-      <c r="Y9" s="7" t="n">
+      <c r="Y10" s="7" t="n">
         <v>1523</v>
       </c>
-      <c r="Z9" s="7" t="n">
+      <c r="Z10" s="7" t="n">
         <v>1651</v>
       </c>
-      <c r="AA9" s="7" t="n">
+      <c r="AA10" s="7" t="n">
         <v>1653</v>
       </c>
-      <c r="AB9" s="7" t="n">
+      <c r="AB10" s="7" t="n">
         <v>1722</v>
       </c>
-      <c r="AC9" s="7" t="n">
+      <c r="AC10" s="7" t="n">
         <v>1723</v>
       </c>
-      <c r="AD9" s="7" t="n">
+      <c r="AD10" s="7" t="n">
         <v>1751</v>
       </c>
-      <c r="AE9" s="7" t="n">
+      <c r="AE10" s="7" t="n">
         <v>1753</v>
       </c>
-      <c r="AF9" s="7" t="n">
+      <c r="AF10" s="7" t="n">
         <v>1851</v>
       </c>
-      <c r="AG9" s="7" t="n">
+      <c r="AG10" s="7" t="n">
         <v>1853</v>
       </c>
-      <c r="AH9" s="7" t="n">
+      <c r="AH10" s="7" t="n">
         <v>2022</v>
       </c>
-      <c r="AI9" s="7" t="n">
+      <c r="AI10" s="7" t="n">
         <v>2023</v>
       </c>
-      <c r="AJ9" s="7" t="n">
+      <c r="AJ10" s="7" t="n">
         <v>2051</v>
       </c>
-      <c r="AK9" s="7" t="n">
+      <c r="AK10" s="7" t="n">
         <v>2053</v>
       </c>
-      <c r="AL9" s="7" t="n">
+      <c r="AL10" s="7" t="n">
         <v>2251</v>
       </c>
-      <c r="AM9" s="7" t="n">
+      <c r="AM10" s="7" t="n">
         <v>2253</v>
       </c>
-      <c r="AN9" s="7" t="n">
+      <c r="AN10" s="7" t="n">
         <v>2351</v>
       </c>
-      <c r="AO9" s="7" t="n">
+      <c r="AO10" s="7" t="n">
         <v>2353</v>
       </c>
-      <c r="AP9" s="7" t="n">
+      <c r="AP10" s="7" t="n">
         <v>2422</v>
       </c>
-      <c r="AQ9" s="7" t="n">
+      <c r="AQ10" s="7" t="n">
         <v>2423</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+    <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="7" t="n">
+      <c r="B11" s="7" t="n">
         <v>728</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C11" s="7" t="n">
         <v>730</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="D11" s="7" t="n">
         <v>758</v>
       </c>
-      <c r="E10" s="7" t="n">
+      <c r="E11" s="7" t="n">
         <v>800</v>
       </c>
-      <c r="F10" s="7" t="n">
+      <c r="F11" s="7" t="n">
         <v>858</v>
       </c>
-      <c r="G10" s="7" t="n">
+      <c r="G11" s="7" t="n">
         <v>900</v>
       </c>
-      <c r="H10" s="7" t="n">
+      <c r="H11" s="7" t="n">
         <v>928</v>
       </c>
-      <c r="I10" s="7" t="n">
+      <c r="I11" s="7" t="n">
         <v>930</v>
       </c>
-      <c r="J10" s="7" t="n">
+      <c r="J11" s="7" t="n">
         <v>958</v>
       </c>
-      <c r="K10" s="7" t="n">
+      <c r="K11" s="7" t="n">
         <v>1000</v>
       </c>
-      <c r="L10" s="7" t="n">
+      <c r="L11" s="7" t="n">
         <v>1058</v>
       </c>
-      <c r="M10" s="7" t="n">
+      <c r="M11" s="7" t="n">
         <v>1100</v>
       </c>
-      <c r="N10" s="7" t="n">
+      <c r="N11" s="7" t="n">
         <v>1128</v>
       </c>
-      <c r="O10" s="7" t="n">
+      <c r="O11" s="7" t="n">
         <v>1130</v>
       </c>
-      <c r="P10" s="7" t="n">
+      <c r="P11" s="7" t="n">
         <v>1158</v>
       </c>
-      <c r="Q10" s="7" t="n">
+      <c r="Q11" s="7" t="n">
         <v>1200</v>
       </c>
-      <c r="R10" s="7" t="n">
+      <c r="R11" s="7" t="n">
         <v>1328</v>
       </c>
-      <c r="S10" s="7" t="n">
+      <c r="S11" s="7" t="n">
         <v>1330</v>
       </c>
-      <c r="T10" s="7" t="n">
+      <c r="T11" s="7" t="n">
         <v>1328</v>
       </c>
-      <c r="U10" s="7" t="n">
+      <c r="U11" s="7" t="n">
         <v>1330</v>
       </c>
-      <c r="V10" s="7" t="n">
+      <c r="V11" s="7" t="n">
         <v>1458</v>
       </c>
-      <c r="W10" s="7" t="n">
+      <c r="W11" s="7" t="n">
         <v>1500</v>
       </c>
-      <c r="X10" s="7" t="n">
+      <c r="X11" s="7" t="n">
         <v>1528</v>
       </c>
-      <c r="Y10" s="7" t="n">
+      <c r="Y11" s="7" t="n">
         <v>1530</v>
       </c>
-      <c r="Z10" s="7" t="n">
+      <c r="Z11" s="7" t="n">
         <v>1658</v>
       </c>
-      <c r="AA10" s="7" t="n">
+      <c r="AA11" s="7" t="n">
         <v>1700</v>
       </c>
-      <c r="AB10" s="7" t="n">
+      <c r="AB11" s="7" t="n">
         <v>1728</v>
       </c>
-      <c r="AC10" s="7" t="n">
+      <c r="AC11" s="7" t="n">
         <v>1730</v>
       </c>
-      <c r="AD10" s="7" t="n">
+      <c r="AD11" s="7" t="n">
         <v>1758</v>
       </c>
-      <c r="AE10" s="7" t="n">
+      <c r="AE11" s="7" t="n">
         <v>1800</v>
       </c>
-      <c r="AF10" s="7" t="n">
+      <c r="AF11" s="7" t="n">
         <v>1858</v>
       </c>
-      <c r="AG10" s="7" t="n">
+      <c r="AG11" s="7" t="n">
         <v>1900</v>
       </c>
-      <c r="AH10" s="7" t="n">
+      <c r="AH11" s="7" t="n">
         <v>2028</v>
       </c>
-      <c r="AI10" s="7" t="n">
+      <c r="AI11" s="7" t="n">
         <v>2030</v>
       </c>
-      <c r="AJ10" s="7" t="n">
+      <c r="AJ11" s="7" t="n">
         <v>2058</v>
       </c>
-      <c r="AK10" s="7" t="n">
+      <c r="AK11" s="7" t="n">
         <v>2100</v>
       </c>
-      <c r="AL10" s="7" t="n">
+      <c r="AL11" s="7" t="n">
         <v>2258</v>
       </c>
-      <c r="AM10" s="7" t="n">
+      <c r="AM11" s="7" t="n">
         <v>2300</v>
       </c>
-      <c r="AN10" s="7" t="n">
+      <c r="AN11" s="7" t="n">
         <v>2400</v>
       </c>
-      <c r="AO10" s="7" t="n">
+      <c r="AO11" s="7" t="n">
         <v>2405</v>
       </c>
-      <c r="AP10" s="7" t="n">
+      <c r="AP11" s="7" t="n">
         <v>2430</v>
       </c>
-      <c r="AQ10" s="7" t="n">
+      <c r="AQ11" s="7" t="n">
         <v>2435</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+    <row r="14" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="3"/>
-      <c r="AC14" s="3"/>
-      <c r="AD14" s="3"/>
-      <c r="AE14" s="3"/>
-      <c r="AF14" s="3"/>
-      <c r="AG14" s="3"/>
-      <c r="AH14" s="3"/>
-      <c r="AI14" s="3"/>
-      <c r="AJ14" s="3"/>
-      <c r="AK14" s="3"/>
-      <c r="AL14" s="3"/>
-      <c r="AM14" s="3"/>
-      <c r="AN14" s="10"/>
-      <c r="AO14" s="10"/>
-      <c r="AP14" s="10"/>
-      <c r="AQ14" s="10"/>
-    </row>
-    <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="3"/>
+      <c r="AJ15" s="3"/>
+      <c r="AK15" s="3"/>
+      <c r="AL15" s="3"/>
+      <c r="AM15" s="3"/>
+      <c r="AN15" s="11"/>
+      <c r="AO15" s="11"/>
+      <c r="AP15" s="11"/>
+      <c r="AQ15" s="11"/>
+    </row>
+    <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="R15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="S15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="T15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="U15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="V15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="W15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="X15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AN15" s="5"/>
-      <c r="AO15" s="5"/>
-      <c r="AP15" s="5"/>
-      <c r="AQ15" s="5"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="7" t="n">
-        <v>531</v>
-      </c>
-      <c r="C16" s="7" t="n">
-        <v>531</v>
-      </c>
-      <c r="D16" s="7" t="n">
-        <v>625</v>
-      </c>
-      <c r="E16" s="7" t="n">
-        <v>630</v>
-      </c>
-      <c r="F16" s="7" t="n">
-        <v>655</v>
-      </c>
-      <c r="G16" s="7" t="n">
-        <v>700</v>
-      </c>
-      <c r="H16" s="7" t="n">
-        <v>755</v>
-      </c>
-      <c r="I16" s="7" t="n">
-        <v>800</v>
-      </c>
-      <c r="J16" s="7" t="n">
-        <v>825</v>
-      </c>
-      <c r="K16" s="7" t="n">
-        <v>830</v>
-      </c>
-      <c r="L16" s="7" t="n">
-        <v>855</v>
-      </c>
-      <c r="M16" s="7" t="n">
-        <v>900</v>
-      </c>
-      <c r="N16" s="7" t="n">
-        <v>1025</v>
-      </c>
-      <c r="O16" s="7" t="n">
-        <v>1030</v>
-      </c>
-      <c r="P16" s="7" t="n">
-        <v>1055</v>
-      </c>
-      <c r="Q16" s="7" t="n">
-        <v>1100</v>
-      </c>
-      <c r="R16" s="7" t="n">
-        <v>1225</v>
-      </c>
-      <c r="S16" s="7" t="n">
-        <v>1230</v>
-      </c>
-      <c r="T16" s="7" t="n">
-        <v>1255</v>
-      </c>
-      <c r="U16" s="7" t="n">
-        <v>1300</v>
-      </c>
-      <c r="V16" s="7" t="n">
-        <v>1355</v>
-      </c>
-      <c r="W16" s="7" t="n">
-        <v>1400</v>
-      </c>
-      <c r="X16" s="7" t="n">
-        <v>1425</v>
-      </c>
-      <c r="Y16" s="7" t="n">
-        <v>1430</v>
-      </c>
-      <c r="Z16" s="7" t="n">
-        <v>1555</v>
-      </c>
-      <c r="AA16" s="7" t="n">
-        <v>1600</v>
-      </c>
-      <c r="AB16" s="7" t="n">
-        <v>1625</v>
-      </c>
-      <c r="AC16" s="7" t="n">
-        <v>1630</v>
-      </c>
-      <c r="AD16" s="7" t="n">
-        <v>1655</v>
-      </c>
-      <c r="AE16" s="7" t="n">
-        <v>1700</v>
-      </c>
-      <c r="AF16" s="7" t="n">
-        <v>1755</v>
-      </c>
-      <c r="AG16" s="7" t="n">
-        <v>1800</v>
-      </c>
-      <c r="AH16" s="7" t="n">
-        <v>1825</v>
-      </c>
-      <c r="AI16" s="7" t="n">
-        <v>1830</v>
-      </c>
-      <c r="AJ16" s="7" t="n">
-        <v>1855</v>
-      </c>
-      <c r="AK16" s="7" t="n">
-        <v>1900</v>
-      </c>
-      <c r="AL16" s="7" t="n">
-        <v>1955</v>
-      </c>
-      <c r="AM16" s="7" t="n">
-        <v>2000</v>
-      </c>
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="W16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN16" s="5"/>
+      <c r="AO16" s="5"/>
+      <c r="AP16" s="5"/>
+      <c r="AQ16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B17" s="7" t="n">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C17" s="7" t="n">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D17" s="7" t="n">
-        <v>633</v>
+        <v>625</v>
       </c>
       <c r="E17" s="7" t="n">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="F17" s="7" t="n">
-        <v>704</v>
+        <v>655</v>
       </c>
       <c r="G17" s="7" t="n">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="H17" s="7" t="n">
-        <v>804</v>
+        <v>755</v>
       </c>
       <c r="I17" s="7" t="n">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="J17" s="7" t="n">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="K17" s="7" t="n">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="L17" s="7" t="n">
-        <v>904</v>
+        <v>855</v>
       </c>
       <c r="M17" s="7" t="n">
-        <v>905</v>
+        <v>900</v>
       </c>
       <c r="N17" s="7" t="n">
-        <v>1033</v>
+        <v>1025</v>
       </c>
       <c r="O17" s="7" t="n">
-        <v>1036</v>
+        <v>1030</v>
       </c>
       <c r="P17" s="7" t="n">
-        <v>1104</v>
+        <v>1055</v>
       </c>
       <c r="Q17" s="7" t="n">
-        <v>1105</v>
+        <v>1100</v>
       </c>
       <c r="R17" s="7" t="n">
-        <v>1233</v>
+        <v>1225</v>
       </c>
       <c r="S17" s="7" t="n">
-        <v>1236</v>
+        <v>1230</v>
       </c>
       <c r="T17" s="7" t="n">
-        <v>1304</v>
+        <v>1255</v>
       </c>
       <c r="U17" s="7" t="n">
-        <v>1305</v>
+        <v>1300</v>
       </c>
       <c r="V17" s="7" t="n">
-        <v>1404</v>
+        <v>1355</v>
       </c>
       <c r="W17" s="7" t="n">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="X17" s="7" t="n">
-        <v>1433</v>
+        <v>1425</v>
       </c>
       <c r="Y17" s="7" t="n">
-        <v>1436</v>
+        <v>1430</v>
       </c>
       <c r="Z17" s="7" t="n">
-        <v>1604</v>
+        <v>1555</v>
       </c>
       <c r="AA17" s="7" t="n">
-        <v>1605</v>
+        <v>1600</v>
       </c>
       <c r="AB17" s="7" t="n">
-        <v>1633</v>
+        <v>1625</v>
       </c>
       <c r="AC17" s="7" t="n">
-        <v>1636</v>
+        <v>1630</v>
       </c>
       <c r="AD17" s="7" t="n">
-        <v>1704</v>
+        <v>1655</v>
       </c>
       <c r="AE17" s="7" t="n">
-        <v>1705</v>
+        <v>1700</v>
       </c>
       <c r="AF17" s="7" t="n">
-        <v>1804</v>
+        <v>1755</v>
       </c>
       <c r="AG17" s="7" t="n">
-        <v>1805</v>
+        <v>1800</v>
       </c>
       <c r="AH17" s="7" t="n">
-        <v>1833</v>
+        <v>1825</v>
       </c>
       <c r="AI17" s="7" t="n">
-        <v>1836</v>
+        <v>1830</v>
       </c>
       <c r="AJ17" s="7" t="n">
-        <v>1904</v>
+        <v>1855</v>
       </c>
       <c r="AK17" s="7" t="n">
-        <v>1905</v>
+        <v>1900</v>
       </c>
       <c r="AL17" s="7" t="n">
-        <v>2004</v>
+        <v>1955</v>
       </c>
       <c r="AM17" s="7" t="n">
-        <v>2005</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="7" t="n">
+        <v>534</v>
+      </c>
+      <c r="C18" s="7" t="n">
+        <v>536</v>
+      </c>
+      <c r="D18" s="7" t="n">
+        <v>633</v>
+      </c>
+      <c r="E18" s="7" t="n">
+        <v>636</v>
+      </c>
+      <c r="F18" s="7" t="n">
+        <v>704</v>
+      </c>
+      <c r="G18" s="7" t="n">
+        <v>705</v>
+      </c>
+      <c r="H18" s="7" t="n">
+        <v>804</v>
+      </c>
+      <c r="I18" s="7" t="n">
+        <v>805</v>
+      </c>
+      <c r="J18" s="7" t="n">
+        <v>833</v>
+      </c>
+      <c r="K18" s="7" t="n">
+        <v>836</v>
+      </c>
+      <c r="L18" s="7" t="n">
+        <v>904</v>
+      </c>
+      <c r="M18" s="7" t="n">
+        <v>905</v>
+      </c>
+      <c r="N18" s="7" t="n">
+        <v>1033</v>
+      </c>
+      <c r="O18" s="7" t="n">
+        <v>1036</v>
+      </c>
+      <c r="P18" s="7" t="n">
+        <v>1104</v>
+      </c>
+      <c r="Q18" s="7" t="n">
+        <v>1105</v>
+      </c>
+      <c r="R18" s="7" t="n">
+        <v>1233</v>
+      </c>
+      <c r="S18" s="7" t="n">
+        <v>1236</v>
+      </c>
+      <c r="T18" s="7" t="n">
+        <v>1304</v>
+      </c>
+      <c r="U18" s="7" t="n">
+        <v>1305</v>
+      </c>
+      <c r="V18" s="7" t="n">
+        <v>1404</v>
+      </c>
+      <c r="W18" s="7" t="n">
+        <v>1405</v>
+      </c>
+      <c r="X18" s="7" t="n">
+        <v>1433</v>
+      </c>
+      <c r="Y18" s="7" t="n">
+        <v>1436</v>
+      </c>
+      <c r="Z18" s="7" t="n">
+        <v>1604</v>
+      </c>
+      <c r="AA18" s="7" t="n">
+        <v>1605</v>
+      </c>
+      <c r="AB18" s="7" t="n">
+        <v>1633</v>
+      </c>
+      <c r="AC18" s="7" t="n">
+        <v>1636</v>
+      </c>
+      <c r="AD18" s="7" t="n">
+        <v>1704</v>
+      </c>
+      <c r="AE18" s="7" t="n">
+        <v>1705</v>
+      </c>
+      <c r="AF18" s="7" t="n">
+        <v>1804</v>
+      </c>
+      <c r="AG18" s="7" t="n">
+        <v>1805</v>
+      </c>
+      <c r="AH18" s="7" t="n">
+        <v>1833</v>
+      </c>
+      <c r="AI18" s="7" t="n">
+        <v>1836</v>
+      </c>
+      <c r="AJ18" s="7" t="n">
+        <v>1904</v>
+      </c>
+      <c r="AK18" s="7" t="n">
+        <v>1905</v>
+      </c>
+      <c r="AL18" s="7" t="n">
+        <v>2004</v>
+      </c>
+      <c r="AM18" s="7" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="7" t="n">
+      <c r="B19" s="7" t="n">
         <v>552</v>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C19" s="7" t="n">
         <v>554</v>
       </c>
-      <c r="D18" s="7" t="n">
+      <c r="D19" s="7" t="n">
         <v>652</v>
       </c>
-      <c r="E18" s="7" t="n">
+      <c r="E19" s="7" t="n">
         <v>654</v>
       </c>
-      <c r="F18" s="7" t="n">
+      <c r="F19" s="7" t="n">
         <v>722</v>
       </c>
-      <c r="G18" s="7" t="n">
+      <c r="G19" s="7" t="n">
         <v>723</v>
       </c>
-      <c r="H18" s="7" t="n">
+      <c r="H19" s="7" t="n">
         <v>822</v>
       </c>
-      <c r="I18" s="7" t="n">
+      <c r="I19" s="7" t="n">
         <v>823</v>
       </c>
-      <c r="J18" s="7" t="n">
+      <c r="J19" s="7" t="n">
         <v>852</v>
       </c>
-      <c r="K18" s="7" t="n">
+      <c r="K19" s="7" t="n">
         <v>854</v>
       </c>
-      <c r="L18" s="7" t="n">
+      <c r="L19" s="7" t="n">
         <v>922</v>
       </c>
-      <c r="M18" s="7" t="n">
+      <c r="M19" s="7" t="n">
         <v>923</v>
       </c>
-      <c r="N18" s="7" t="n">
+      <c r="N19" s="7" t="n">
         <v>1052</v>
       </c>
-      <c r="O18" s="7" t="n">
+      <c r="O19" s="7" t="n">
         <v>1054</v>
       </c>
-      <c r="P18" s="7" t="n">
+      <c r="P19" s="7" t="n">
         <v>1122</v>
       </c>
-      <c r="Q18" s="7" t="n">
+      <c r="Q19" s="7" t="n">
         <v>1123</v>
       </c>
-      <c r="R18" s="7" t="n">
+      <c r="R19" s="7" t="n">
         <v>1252</v>
       </c>
-      <c r="S18" s="7" t="n">
+      <c r="S19" s="7" t="n">
         <v>1254</v>
       </c>
-      <c r="T18" s="7" t="n">
+      <c r="T19" s="7" t="n">
         <v>1322</v>
       </c>
-      <c r="U18" s="7" t="n">
+      <c r="U19" s="7" t="n">
         <v>1323</v>
       </c>
-      <c r="V18" s="7" t="n">
+      <c r="V19" s="7" t="n">
         <v>1422</v>
       </c>
-      <c r="W18" s="7" t="n">
+      <c r="W19" s="7" t="n">
         <v>1423</v>
       </c>
-      <c r="X18" s="7" t="n">
+      <c r="X19" s="7" t="n">
         <v>1452</v>
       </c>
-      <c r="Y18" s="7" t="n">
+      <c r="Y19" s="7" t="n">
         <v>1454</v>
       </c>
-      <c r="Z18" s="7" t="n">
+      <c r="Z19" s="7" t="n">
         <v>1622</v>
       </c>
-      <c r="AA18" s="7" t="n">
+      <c r="AA19" s="7" t="n">
         <v>1623</v>
       </c>
-      <c r="AB18" s="7" t="n">
+      <c r="AB19" s="7" t="n">
         <v>1652</v>
       </c>
-      <c r="AC18" s="7" t="n">
+      <c r="AC19" s="7" t="n">
         <v>1654</v>
       </c>
-      <c r="AD18" s="7" t="n">
+      <c r="AD19" s="7" t="n">
         <v>1722</v>
       </c>
-      <c r="AE18" s="7" t="n">
+      <c r="AE19" s="7" t="n">
         <v>1723</v>
       </c>
-      <c r="AF18" s="7" t="n">
+      <c r="AF19" s="7" t="n">
         <v>1822</v>
       </c>
-      <c r="AG18" s="7" t="n">
+      <c r="AG19" s="7" t="n">
         <v>1823</v>
       </c>
-      <c r="AH18" s="7" t="n">
+      <c r="AH19" s="7" t="n">
         <v>1852</v>
       </c>
-      <c r="AI18" s="7" t="n">
+      <c r="AI19" s="7" t="n">
         <v>1854</v>
       </c>
-      <c r="AJ18" s="7" t="n">
+      <c r="AJ19" s="7" t="n">
         <v>1922</v>
       </c>
-      <c r="AK18" s="7" t="n">
+      <c r="AK19" s="7" t="n">
         <v>1923</v>
       </c>
-      <c r="AL18" s="7" t="n">
+      <c r="AL19" s="7" t="n">
         <v>2022</v>
       </c>
-      <c r="AM18" s="7" t="n">
+      <c r="AM19" s="7" t="n">
         <v>2023</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+    <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="7" t="n">
+      <c r="B20" s="7" t="n">
         <v>603</v>
       </c>
-      <c r="C19" s="7" t="n">
+      <c r="C20" s="7" t="n">
         <v>604</v>
       </c>
-      <c r="D19" s="7" t="n">
+      <c r="D20" s="7" t="n">
         <v>703</v>
       </c>
-      <c r="E19" s="7" t="n">
+      <c r="E20" s="7" t="n">
         <v>704</v>
       </c>
-      <c r="F19" s="7" t="n">
+      <c r="F20" s="7" t="n">
         <v>732</v>
       </c>
-      <c r="G19" s="7" t="n">
+      <c r="G20" s="7" t="n">
         <v>733</v>
       </c>
-      <c r="H19" s="7" t="n">
+      <c r="H20" s="7" t="n">
         <v>832</v>
       </c>
-      <c r="I19" s="7" t="n">
+      <c r="I20" s="7" t="n">
         <v>833</v>
       </c>
-      <c r="J19" s="7" t="n">
+      <c r="J20" s="7" t="n">
         <v>903</v>
       </c>
-      <c r="K19" s="7" t="n">
+      <c r="K20" s="7" t="n">
         <v>904</v>
       </c>
-      <c r="L19" s="7" t="n">
+      <c r="L20" s="7" t="n">
         <v>932</v>
       </c>
-      <c r="M19" s="7" t="n">
+      <c r="M20" s="7" t="n">
         <v>933</v>
       </c>
-      <c r="N19" s="7" t="n">
+      <c r="N20" s="7" t="n">
         <v>1103</v>
       </c>
-      <c r="O19" s="7" t="n">
+      <c r="O20" s="7" t="n">
         <v>1104</v>
       </c>
-      <c r="P19" s="7" t="n">
+      <c r="P20" s="7" t="n">
         <v>1132</v>
       </c>
-      <c r="Q19" s="7" t="n">
+      <c r="Q20" s="7" t="n">
         <v>1133</v>
       </c>
-      <c r="R19" s="7" t="n">
+      <c r="R20" s="7" t="n">
         <v>1303</v>
       </c>
-      <c r="S19" s="7" t="n">
+      <c r="S20" s="7" t="n">
         <v>1304</v>
       </c>
-      <c r="T19" s="7" t="n">
+      <c r="T20" s="7" t="n">
         <v>1332</v>
       </c>
-      <c r="U19" s="7" t="n">
+      <c r="U20" s="7" t="n">
         <v>1333</v>
       </c>
-      <c r="V19" s="7" t="n">
+      <c r="V20" s="7" t="n">
         <v>1432</v>
       </c>
-      <c r="W19" s="7" t="n">
+      <c r="W20" s="7" t="n">
         <v>1433</v>
       </c>
-      <c r="X19" s="7" t="n">
+      <c r="X20" s="7" t="n">
         <v>1503</v>
       </c>
-      <c r="Y19" s="7" t="n">
+      <c r="Y20" s="7" t="n">
         <v>1504</v>
       </c>
-      <c r="Z19" s="7" t="n">
+      <c r="Z20" s="7" t="n">
         <v>1632</v>
       </c>
-      <c r="AA19" s="7" t="n">
+      <c r="AA20" s="7" t="n">
         <v>1633</v>
       </c>
-      <c r="AB19" s="7" t="n">
+      <c r="AB20" s="7" t="n">
         <v>1703</v>
       </c>
-      <c r="AC19" s="7" t="n">
+      <c r="AC20" s="7" t="n">
         <v>1704</v>
       </c>
-      <c r="AD19" s="7" t="n">
+      <c r="AD20" s="7" t="n">
         <v>1732</v>
       </c>
-      <c r="AE19" s="7" t="n">
+      <c r="AE20" s="7" t="n">
         <v>1733</v>
       </c>
-      <c r="AF19" s="7" t="n">
+      <c r="AF20" s="7" t="n">
         <v>1832</v>
       </c>
-      <c r="AG19" s="7" t="n">
+      <c r="AG20" s="7" t="n">
         <v>1833</v>
       </c>
-      <c r="AH19" s="7" t="n">
+      <c r="AH20" s="7" t="n">
         <v>1903</v>
       </c>
-      <c r="AI19" s="7" t="n">
+      <c r="AI20" s="7" t="n">
         <v>1904</v>
       </c>
-      <c r="AJ19" s="7" t="n">
+      <c r="AJ20" s="7" t="n">
         <v>1932</v>
       </c>
-      <c r="AK19" s="7" t="n">
+      <c r="AK20" s="7" t="n">
         <v>1933</v>
       </c>
-      <c r="AL19" s="7" t="n">
+      <c r="AL20" s="7" t="n">
         <v>2032</v>
       </c>
-      <c r="AM19" s="7" t="n">
+      <c r="AM20" s="7" t="n">
         <v>2033</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="7" t="n">
+      <c r="B21" s="7" t="n">
         <v>624</v>
       </c>
-      <c r="C20" s="7" t="n">
+      <c r="C21" s="7" t="n">
         <v>636</v>
       </c>
-      <c r="D20" s="7" t="n">
+      <c r="D21" s="7" t="n">
         <v>724</v>
       </c>
-      <c r="E20" s="7" t="n">
+      <c r="E21" s="7" t="n">
         <v>736</v>
       </c>
-      <c r="F20" s="7" t="n">
+      <c r="F21" s="7" t="n">
         <v>752</v>
       </c>
-      <c r="G20" s="7" t="n">
+      <c r="G21" s="7" t="n">
         <v>804</v>
       </c>
-      <c r="H20" s="7" t="n">
+      <c r="H21" s="7" t="n">
         <v>852</v>
       </c>
-      <c r="I20" s="7" t="n">
+      <c r="I21" s="7" t="n">
         <v>904</v>
       </c>
-      <c r="J20" s="7" t="n">
+      <c r="J21" s="7" t="n">
         <v>924</v>
       </c>
-      <c r="K20" s="7" t="n">
+      <c r="K21" s="7" t="n">
         <v>936</v>
       </c>
-      <c r="L20" s="7" t="n">
+      <c r="L21" s="7" t="n">
         <v>952</v>
       </c>
-      <c r="M20" s="7" t="n">
+      <c r="M21" s="7" t="n">
         <v>1004</v>
       </c>
-      <c r="N20" s="7" t="n">
+      <c r="N21" s="7" t="n">
         <v>1124</v>
       </c>
-      <c r="O20" s="7" t="n">
+      <c r="O21" s="7" t="n">
         <v>1136</v>
       </c>
-      <c r="P20" s="7" t="n">
+      <c r="P21" s="7" t="n">
         <v>1152</v>
       </c>
-      <c r="Q20" s="7" t="n">
+      <c r="Q21" s="7" t="n">
         <v>1204</v>
       </c>
-      <c r="R20" s="7" t="n">
+      <c r="R21" s="7" t="n">
         <v>1324</v>
       </c>
-      <c r="S20" s="7" t="n">
+      <c r="S21" s="7" t="n">
         <v>1336</v>
       </c>
-      <c r="T20" s="7" t="n">
+      <c r="T21" s="7" t="n">
         <v>1352</v>
       </c>
-      <c r="U20" s="7" t="n">
+      <c r="U21" s="7" t="n">
         <v>1404</v>
       </c>
-      <c r="V20" s="7" t="n">
+      <c r="V21" s="7" t="n">
         <v>1452</v>
       </c>
-      <c r="W20" s="7" t="n">
+      <c r="W21" s="7" t="n">
         <v>1504</v>
       </c>
-      <c r="X20" s="7" t="n">
+      <c r="X21" s="7" t="n">
         <v>1524</v>
       </c>
-      <c r="Y20" s="7" t="n">
+      <c r="Y21" s="7" t="n">
         <v>1536</v>
       </c>
-      <c r="Z20" s="7" t="n">
+      <c r="Z21" s="7" t="n">
         <v>1652</v>
       </c>
-      <c r="AA20" s="7" t="n">
+      <c r="AA21" s="7" t="n">
         <v>1704</v>
       </c>
-      <c r="AB20" s="7" t="n">
+      <c r="AB21" s="7" t="n">
         <v>1724</v>
       </c>
-      <c r="AC20" s="7" t="n">
+      <c r="AC21" s="7" t="n">
         <v>1736</v>
       </c>
-      <c r="AD20" s="7" t="n">
+      <c r="AD21" s="7" t="n">
         <v>1752</v>
       </c>
-      <c r="AE20" s="7" t="n">
+      <c r="AE21" s="7" t="n">
         <v>1804</v>
       </c>
-      <c r="AF20" s="7" t="n">
+      <c r="AF21" s="7" t="n">
         <v>1852</v>
       </c>
-      <c r="AG20" s="7" t="n">
+      <c r="AG21" s="7" t="n">
         <v>1904</v>
       </c>
-      <c r="AH20" s="7" t="n">
+      <c r="AH21" s="7" t="n">
         <v>1924</v>
       </c>
-      <c r="AI20" s="7" t="n">
+      <c r="AI21" s="7" t="n">
         <v>1936</v>
       </c>
-      <c r="AJ20" s="7" t="n">
+      <c r="AJ21" s="7" t="n">
         <v>1952</v>
       </c>
-      <c r="AK20" s="7" t="n">
+      <c r="AK21" s="7" t="n">
         <v>2004</v>
       </c>
-      <c r="AL20" s="7" t="n">
+      <c r="AL21" s="7" t="n">
         <v>2052</v>
       </c>
-      <c r="AM20" s="7" t="n">
+      <c r="AM21" s="7" t="n">
         <v>2104</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+    <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="7" t="n">
+      <c r="B22" s="7" t="n">
         <v>703</v>
       </c>
-      <c r="C21" s="7" t="n">
+      <c r="C22" s="7" t="n">
         <v>705</v>
       </c>
-      <c r="D21" s="7" t="n">
+      <c r="D22" s="7" t="n">
         <v>803</v>
       </c>
-      <c r="E21" s="7" t="n">
+      <c r="E22" s="7" t="n">
         <v>805</v>
       </c>
-      <c r="F21" s="7" t="n">
+      <c r="F22" s="7" t="n">
         <v>830</v>
       </c>
-      <c r="G21" s="7" t="n">
+      <c r="G22" s="7" t="n">
         <v>833</v>
       </c>
-      <c r="H21" s="7" t="n">
+      <c r="H22" s="7" t="n">
         <v>930</v>
       </c>
-      <c r="I21" s="7" t="n">
+      <c r="I22" s="7" t="n">
         <v>933</v>
       </c>
-      <c r="J21" s="7" t="n">
+      <c r="J22" s="7" t="n">
         <v>1003</v>
       </c>
-      <c r="K21" s="7" t="n">
+      <c r="K22" s="7" t="n">
         <v>1005</v>
       </c>
-      <c r="L21" s="7" t="n">
+      <c r="L22" s="7" t="n">
         <v>1030</v>
       </c>
-      <c r="M21" s="7" t="n">
+      <c r="M22" s="7" t="n">
         <v>1033</v>
       </c>
-      <c r="N21" s="7" t="n">
+      <c r="N22" s="7" t="n">
         <v>1203</v>
       </c>
-      <c r="O21" s="7" t="n">
+      <c r="O22" s="7" t="n">
         <v>1205</v>
       </c>
-      <c r="P21" s="7" t="n">
+      <c r="P22" s="7" t="n">
         <v>1230</v>
       </c>
-      <c r="Q21" s="7" t="n">
+      <c r="Q22" s="7" t="n">
         <v>1233</v>
       </c>
-      <c r="R21" s="7" t="n">
+      <c r="R22" s="7" t="n">
         <v>1403</v>
       </c>
-      <c r="S21" s="7" t="n">
+      <c r="S22" s="7" t="n">
         <v>1405</v>
       </c>
-      <c r="T21" s="7" t="n">
+      <c r="T22" s="7" t="n">
         <v>1430</v>
       </c>
-      <c r="U21" s="7" t="n">
+      <c r="U22" s="7" t="n">
         <v>1433</v>
       </c>
-      <c r="V21" s="7" t="n">
+      <c r="V22" s="7" t="n">
         <v>1530</v>
       </c>
-      <c r="W21" s="7" t="n">
+      <c r="W22" s="7" t="n">
         <v>1533</v>
       </c>
-      <c r="X21" s="7" t="n">
+      <c r="X22" s="7" t="n">
         <v>1603</v>
       </c>
-      <c r="Y21" s="7" t="n">
+      <c r="Y22" s="7" t="n">
         <v>1605</v>
       </c>
-      <c r="Z21" s="7" t="n">
+      <c r="Z22" s="7" t="n">
         <v>1730</v>
       </c>
-      <c r="AA21" s="7" t="n">
+      <c r="AA22" s="7" t="n">
         <v>1733</v>
       </c>
-      <c r="AB21" s="7" t="n">
+      <c r="AB22" s="7" t="n">
         <v>1803</v>
       </c>
-      <c r="AC21" s="7" t="n">
+      <c r="AC22" s="7" t="n">
         <v>1805</v>
       </c>
-      <c r="AD21" s="7" t="n">
+      <c r="AD22" s="7" t="n">
         <v>1830</v>
       </c>
-      <c r="AE21" s="7" t="n">
+      <c r="AE22" s="7" t="n">
         <v>1833</v>
       </c>
-      <c r="AF21" s="7" t="n">
+      <c r="AF22" s="7" t="n">
         <v>1930</v>
       </c>
-      <c r="AG21" s="7" t="n">
+      <c r="AG22" s="7" t="n">
         <v>1933</v>
       </c>
-      <c r="AH21" s="7" t="n">
+      <c r="AH22" s="7" t="n">
         <v>2003</v>
       </c>
-      <c r="AI21" s="7" t="n">
+      <c r="AI22" s="7" t="n">
         <v>2005</v>
       </c>
-      <c r="AJ21" s="7" t="n">
+      <c r="AJ22" s="7" t="n">
         <v>2030</v>
       </c>
-      <c r="AK21" s="7" t="n">
+      <c r="AK22" s="7" t="n">
         <v>2033</v>
       </c>
-      <c r="AL21" s="7" t="n">
+      <c r="AL22" s="7" t="n">
         <v>2130</v>
       </c>
-      <c r="AM21" s="7" t="n">
+      <c r="AM22" s="7" t="n">
         <v>2133</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7" t="n">
-        <v>849</v>
-      </c>
-      <c r="G22" s="7" t="n">
-        <v>850</v>
-      </c>
-      <c r="H22" s="7" t="n">
-        <v>949</v>
-      </c>
-      <c r="I22" s="7" t="n">
-        <v>950</v>
-      </c>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7" t="n">
-        <v>1049</v>
-      </c>
-      <c r="M22" s="7" t="n">
-        <v>1050</v>
-      </c>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7" t="n">
-        <v>1249</v>
-      </c>
-      <c r="Q22" s="7" t="n">
-        <v>1250</v>
-      </c>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7" t="n">
-        <v>1449</v>
-      </c>
-      <c r="U22" s="7" t="n">
-        <v>1450</v>
-      </c>
-      <c r="V22" s="7" t="n">
-        <v>1549</v>
-      </c>
-      <c r="W22" s="7" t="n">
-        <v>1550</v>
-      </c>
-      <c r="X22" s="7"/>
-      <c r="Y22" s="7"/>
-      <c r="Z22" s="7" t="n">
-        <v>1749</v>
-      </c>
-      <c r="AA22" s="7" t="n">
-        <v>1750</v>
-      </c>
-      <c r="AB22" s="7"/>
-      <c r="AC22" s="7"/>
-      <c r="AD22" s="7" t="n">
-        <v>1849</v>
-      </c>
-      <c r="AE22" s="7" t="n">
-        <v>1850</v>
-      </c>
-      <c r="AF22" s="7" t="n">
-        <v>1949</v>
-      </c>
-      <c r="AG22" s="7" t="n">
-        <v>1950</v>
-      </c>
-      <c r="AH22" s="7"/>
-      <c r="AI22" s="7"/>
-      <c r="AJ22" s="7" t="n">
-        <v>2049</v>
-      </c>
-      <c r="AK22" s="7" t="n">
-        <v>2050</v>
-      </c>
-      <c r="AL22" s="7" t="n">
-        <v>2149</v>
-      </c>
-      <c r="AM22" s="7" t="n">
-        <v>2150</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7" t="n">
+        <v>849</v>
+      </c>
+      <c r="G23" s="7" t="n">
+        <v>850</v>
+      </c>
+      <c r="H23" s="7" t="n">
+        <v>949</v>
+      </c>
+      <c r="I23" s="7" t="n">
+        <v>950</v>
+      </c>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7" t="n">
+        <v>1049</v>
+      </c>
+      <c r="M23" s="7" t="n">
+        <v>1050</v>
+      </c>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7" t="n">
+        <v>1249</v>
+      </c>
+      <c r="Q23" s="7" t="n">
+        <v>1250</v>
+      </c>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7" t="n">
+        <v>1449</v>
+      </c>
+      <c r="U23" s="7" t="n">
+        <v>1450</v>
+      </c>
+      <c r="V23" s="7" t="n">
+        <v>1549</v>
+      </c>
+      <c r="W23" s="7" t="n">
+        <v>1550</v>
+      </c>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7" t="n">
+        <v>1749</v>
+      </c>
+      <c r="AA23" s="7" t="n">
+        <v>1750</v>
+      </c>
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7" t="n">
+        <v>1849</v>
+      </c>
+      <c r="AE23" s="7" t="n">
+        <v>1850</v>
+      </c>
+      <c r="AF23" s="7" t="n">
+        <v>1949</v>
+      </c>
+      <c r="AG23" s="7" t="n">
+        <v>1950</v>
+      </c>
+      <c r="AH23" s="7"/>
+      <c r="AI23" s="7"/>
+      <c r="AJ23" s="7" t="n">
+        <v>2049</v>
+      </c>
+      <c r="AK23" s="7" t="n">
+        <v>2050</v>
+      </c>
+      <c r="AL23" s="7" t="n">
+        <v>2149</v>
+      </c>
+      <c r="AM23" s="7" t="n">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="7" t="n">
+      <c r="B24" s="7" t="n">
         <v>732</v>
       </c>
-      <c r="C23" s="7" t="n">
+      <c r="C24" s="7" t="n">
         <v>735</v>
       </c>
-      <c r="D23" s="7" t="n">
+      <c r="D24" s="7" t="n">
         <v>832</v>
       </c>
-      <c r="E23" s="7" t="n">
+      <c r="E24" s="7" t="n">
         <v>835</v>
       </c>
-      <c r="F23" s="7" t="n">
+      <c r="F24" s="7" t="n">
         <v>901</v>
       </c>
-      <c r="G23" s="7" t="n">
+      <c r="G24" s="7" t="n">
         <v>905</v>
       </c>
-      <c r="H23" s="7" t="n">
+      <c r="H24" s="7" t="n">
         <v>1001</v>
       </c>
-      <c r="I23" s="7" t="n">
+      <c r="I24" s="7" t="n">
         <v>1005</v>
       </c>
-      <c r="J23" s="7" t="n">
+      <c r="J24" s="7" t="n">
         <v>1032</v>
       </c>
-      <c r="K23" s="7" t="n">
+      <c r="K24" s="7" t="n">
         <v>1035</v>
       </c>
-      <c r="L23" s="7" t="n">
+      <c r="L24" s="7" t="n">
         <v>1101</v>
       </c>
-      <c r="M23" s="7" t="n">
+      <c r="M24" s="7" t="n">
         <v>1105</v>
       </c>
-      <c r="N23" s="7" t="n">
+      <c r="N24" s="7" t="n">
         <v>1232</v>
       </c>
-      <c r="O23" s="7" t="n">
+      <c r="O24" s="7" t="n">
         <v>1235</v>
       </c>
-      <c r="P23" s="7" t="n">
+      <c r="P24" s="7" t="n">
         <v>1301</v>
       </c>
-      <c r="Q23" s="7" t="n">
+      <c r="Q24" s="7" t="n">
         <v>1305</v>
       </c>
-      <c r="R23" s="7" t="n">
+      <c r="R24" s="7" t="n">
         <v>1432</v>
       </c>
-      <c r="S23" s="7" t="n">
+      <c r="S24" s="7" t="n">
         <v>1435</v>
       </c>
-      <c r="T23" s="7" t="n">
+      <c r="T24" s="7" t="n">
         <v>1501</v>
       </c>
-      <c r="U23" s="7" t="n">
+      <c r="U24" s="7" t="n">
         <v>1505</v>
       </c>
-      <c r="V23" s="7" t="n">
+      <c r="V24" s="7" t="n">
         <v>1601</v>
       </c>
-      <c r="W23" s="7" t="n">
+      <c r="W24" s="7" t="n">
         <v>1605</v>
       </c>
-      <c r="X23" s="7" t="n">
+      <c r="X24" s="7" t="n">
         <v>1632</v>
       </c>
-      <c r="Y23" s="7" t="n">
+      <c r="Y24" s="7" t="n">
         <v>1635</v>
       </c>
-      <c r="Z23" s="7" t="n">
+      <c r="Z24" s="7" t="n">
         <v>1801</v>
       </c>
-      <c r="AA23" s="7" t="n">
+      <c r="AA24" s="7" t="n">
         <v>1805</v>
       </c>
-      <c r="AB23" s="7" t="n">
+      <c r="AB24" s="7" t="n">
         <v>1832</v>
       </c>
-      <c r="AC23" s="7" t="n">
+      <c r="AC24" s="7" t="n">
         <v>1835</v>
       </c>
-      <c r="AD23" s="7" t="n">
+      <c r="AD24" s="7" t="n">
         <v>1901</v>
       </c>
-      <c r="AE23" s="7" t="n">
+      <c r="AE24" s="7" t="n">
         <v>1905</v>
       </c>
-      <c r="AF23" s="7" t="n">
+      <c r="AF24" s="7" t="n">
         <v>2001</v>
       </c>
-      <c r="AG23" s="7" t="n">
+      <c r="AG24" s="7" t="n">
         <v>2005</v>
       </c>
-      <c r="AH23" s="7" t="n">
+      <c r="AH24" s="7" t="n">
         <v>2032</v>
       </c>
-      <c r="AI23" s="7" t="n">
+      <c r="AI24" s="7" t="n">
         <v>2035</v>
       </c>
-      <c r="AJ23" s="7" t="n">
+      <c r="AJ24" s="7" t="n">
         <v>2101</v>
       </c>
-      <c r="AK23" s="7" t="n">
+      <c r="AK24" s="7" t="n">
         <v>2105</v>
       </c>
-      <c r="AL23" s="7" t="n">
+      <c r="AL24" s="7" t="n">
         <v>2201</v>
       </c>
-      <c r="AM23" s="7" t="n">
+      <c r="AM24" s="7" t="n">
         <v>2205</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:AQ1"/>
-    <mergeCell ref="A14:AM14"/>
+    <mergeCell ref="A2:AQ2"/>
+    <mergeCell ref="A15:AM15"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -14489,7 +14556,7 @@
   <dimension ref="A1:AL22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AL2" activeCellId="0" sqref="AL2"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>